<commit_message>
doc: RMMM Tabelle aktualisiert
</commit_message>
<xml_diff>
--- a/documentation/RMMM_Risiken_Restaurantprojekt.xlsx
+++ b/documentation/RMMM_Risiken_Restaurantprojekt.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unlqvt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\source\repos\SoftwareEngineeringProjektTINF23B5\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B52FBE-5D45-48DF-BAA0-3421B68EEE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Risk ID</t>
   </si>
@@ -97,9 +98,6 @@
   </si>
   <si>
     <t>Scrum Master</t>
-  </si>
-  <si>
-    <t>Offen</t>
   </si>
   <si>
     <t>09.04.2025</t>
@@ -180,7 +178,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,12 +231,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -257,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -297,9 +303,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -334,7 +340,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,7 +375,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -542,26 +548,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="112.28515625" customWidth="1"/>
-    <col min="7" max="7" width="80.28515625" customWidth="1"/>
-    <col min="8" max="8" width="101.5703125" customWidth="1"/>
-    <col min="9" max="9" width="179.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="112.265625" customWidth="1"/>
+    <col min="7" max="7" width="80.265625" customWidth="1"/>
+    <col min="8" max="8" width="101.59765625" customWidth="1"/>
+    <col min="9" max="9" width="179.73046875" customWidth="1"/>
+    <col min="10" max="10" width="24.265625" customWidth="1"/>
+    <col min="11" max="11" width="15.1328125" customWidth="1"/>
+    <col min="12" max="12" width="17.46484375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,11 +601,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -607,7 +613,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -631,13 +637,13 @@
         <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -645,7 +651,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -669,21 +675,21 @@
         <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="L3" s="4">
+        <v>45812</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -695,36 +701,36 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" t="s">
-        <v>35</v>
-      </c>
       <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
         <v>37</v>
       </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="2">
-        <v>45757</v>
+      <c r="L4" s="4">
+        <v>45822</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
@@ -733,36 +739,36 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="4">
+        <v>45812</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="2">
-        <v>45757</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -771,22 +777,22 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>49</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>50</v>
       </c>
-      <c r="J6" t="s">
-        <v>51</v>
-      </c>
       <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="2">
-        <v>45757</v>
+        <v>37</v>
+      </c>
+      <c r="L6" s="4">
+        <v>45823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>